<commit_message>
Another round of figure setting
</commit_message>
<xml_diff>
--- a/output/supp_mat2.xlsx
+++ b/output/supp_mat2.xlsx
@@ -1,122 +1,121 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgilbe01\Desktop\PhD_2020-2023_09\01.Analyses\FeSthOpinn\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F67704B-1585-49EF-B30B-654DEF6A7A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Nb of days of presence considered in the study</t>
-  </si>
-  <si>
-    <t>Mean Fe yearly release (t/yr)</t>
-  </si>
-  <si>
-    <t>Confidence interval</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Sperm whales</t>
-  </si>
-  <si>
-    <t>365</t>
-  </si>
-  <si>
-    <t>Lavery et al. 2010</t>
-  </si>
-  <si>
-    <t>Antarctic blue whales</t>
-  </si>
-  <si>
-    <t>Lavery et al. 2014</t>
-  </si>
-  <si>
-    <t>60-180</t>
-  </si>
-  <si>
-    <t>9-24</t>
-  </si>
-  <si>
-    <t>Savoca et al. 2021</t>
-  </si>
-  <si>
-    <t>Humpback whales</t>
-  </si>
-  <si>
-    <t>144-394</t>
-  </si>
-  <si>
-    <t>Antarctic fin whales</t>
-  </si>
-  <si>
-    <t>193-590</t>
-  </si>
-  <si>
-    <t>Antarctic minke whales</t>
-  </si>
-  <si>
-    <t>420-937</t>
-  </si>
-  <si>
-    <t>Chinstrap, Adelie and Gentoo penguins</t>
-  </si>
-  <si>
-    <t>deduced from Sparaventi et al. 2021</t>
-  </si>
-  <si>
-    <t>Leopard seals</t>
-  </si>
-  <si>
-    <t>2.3 - 24.8</t>
-  </si>
-  <si>
-    <t>this study</t>
-  </si>
-  <si>
-    <t>Weddell seals</t>
-  </si>
-  <si>
-    <t>12.5 - 105.2</t>
-  </si>
-  <si>
-    <t>Crabeater seals</t>
-  </si>
-  <si>
-    <t>59.8 - 316</t>
-  </si>
-  <si>
-    <t>Ross seals</t>
-  </si>
-  <si>
-    <t>0.9 - 7.6</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t xml:space="preserve">Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nb of days of presence considered in the study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean Fe yearly release (t/yr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confidence interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sperm whales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lavery et al. 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antarctic blue whales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lavery et al. 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60-180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Savoca et al. 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Humpback whales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">144-394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antarctic fin whales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">193-590</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antarctic minke whales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">420-937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chinstrap, Adelie and Gentoo penguins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deduced from Sparaventi et al. 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimates from this study were originally calculated for the reproduction period only. They were raised to annual estimates using a simple cross product.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leopard seals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3 - 24.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weddell seals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.5 - 105.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crabeater seals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59.8 - 316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ross seals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9 - 7.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -152,15 +151,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -442,20 +432,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.1796875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,187 +455,206 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
         <v>50</v>
       </c>
+      <c r="D2"/>
       <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>65</v>
       </c>
+      <c r="D3"/>
       <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="C4" t="n">
         <v>15</v>
       </c>
       <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="C5" t="n">
+        <v>221</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>221</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5"/>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="C6" t="n">
         <v>367</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="F6"/>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="C7" t="n">
         <v>630</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="F7"/>
+    </row>
+    <row r="8">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
         <v>169</v>
       </c>
+      <c r="D8"/>
       <c r="E8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
         <v>9.9</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="F9"/>
+    </row>
+    <row r="10">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="C10" t="n">
         <v>44.1</v>
       </c>
       <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10"/>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="n">
         <v>151.5</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="F11"/>
+    </row>
+    <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="C12" t="n">
         <v>3.1</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>